<commit_message>
add percentage in result form
</commit_message>
<xml_diff>
--- a/PMS/forms/result_form.xlsx
+++ b/PMS/forms/result_form.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TRƯỜNG ĐH QUỐC TẾ MIỀN ĐÔNG</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>NGÀNH CÔNG NGHỆ THÔNG TIN</t>
+  </si>
+  <si>
+    <t>Tỉ lệ điểm (%)</t>
+  </si>
+  <si>
+    <t>Điểm chữ:</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -198,6 +204,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -504,108 +513,119 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" customWidth="1"/>
+    <col min="3" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>2</v>
@@ -613,50 +633,57 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>3</v>
@@ -664,8 +691,9 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="7" t="s">
         <v>4</v>
@@ -674,60 +702,78 @@
         <v>7</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="8"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="C8:E10"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A5:E5"/>
+  <mergeCells count="8">
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="C8:F10"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="70" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>